<commit_message>
Add merge function but not complete
</commit_message>
<xml_diff>
--- a/studMin/TemplateExcel/subject.xlsx
+++ b/studMin/TemplateExcel/subject.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Khoi\Documents\GitHub\studMin\studMin\TemplateExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B2E9D9-E53D-41E7-AA61-C56B1476C213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876D9AAE-552E-4310-AEC2-631E00759DDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>BẢNG ĐIỂM MÔN NGỮ VĂN</t>
   </si>
@@ -59,27 +59,6 @@
   </si>
   <si>
     <t>Nguyễn Văn An</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>9.5</t>
-  </si>
-  <si>
-    <t>9.75</t>
-  </si>
-  <si>
-    <t>Trần Thanh Tú</t>
-  </si>
-  <si>
-    <t>Lý Văn Hưng</t>
   </si>
 </sst>
 </file>
@@ -660,7 +639,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+      <selection pane="bottomLeft" activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -783,133 +762,59 @@
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="5"/>
-      <c r="M6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="P6" s="22">
-        <v>10</v>
-      </c>
-      <c r="Q6" s="8">
-        <v>9.1</v>
-      </c>
+      <c r="M6" s="3"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="8"/>
     </row>
     <row r="7" spans="1:17" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>2</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="1">
-        <v>10</v>
-      </c>
-      <c r="E7" s="1">
-        <v>9</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="7"/>
-      <c r="H7" s="8">
-        <v>9</v>
-      </c>
-      <c r="I7" s="1">
-        <v>7</v>
-      </c>
-      <c r="J7" s="1">
-        <v>8.5</v>
-      </c>
+      <c r="H7" s="8"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="7"/>
-      <c r="M7" s="9">
-        <v>10</v>
-      </c>
-      <c r="N7" s="1">
-        <v>8</v>
-      </c>
-      <c r="O7" s="7">
-        <v>9.75</v>
-      </c>
-      <c r="P7" s="22">
-        <v>10</v>
-      </c>
-      <c r="Q7" s="8">
-        <v>9.5</v>
-      </c>
+      <c r="M7" s="9"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="8"/>
     </row>
     <row r="8" spans="1:17" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>3</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="1">
-        <v>8</v>
-      </c>
-      <c r="E8" s="1">
-        <v>9</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="7"/>
-      <c r="H8" s="8">
-        <v>7</v>
-      </c>
-      <c r="I8" s="1">
-        <v>8</v>
-      </c>
-      <c r="J8" s="1">
-        <v>9.5</v>
-      </c>
+      <c r="H8" s="8"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="7"/>
-      <c r="M8" s="9">
-        <v>10</v>
-      </c>
-      <c r="N8" s="1">
-        <v>8</v>
-      </c>
-      <c r="O8" s="7">
-        <v>8.5</v>
-      </c>
-      <c r="P8" s="22">
-        <v>10</v>
-      </c>
-      <c r="Q8" s="8">
-        <v>9.5</v>
-      </c>
+      <c r="M8" s="9"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="8"/>
     </row>
     <row r="9" spans="1:17" ht="16.8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>

</xml_diff>